<commit_message>
add hpc partition to uva cpu sensitivity analysis
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/benchmarking_uva_cpus.xlsx
+++ b/test_data/norfolk_coastal_flooding/benchmarking_uva_cpus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CAA417-4FC9-4EA4-9757-9181572D5F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E60E24-89CF-4711-BC12-46A058228C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="23">
   <si>
     <t>hardware_utilization_strategy</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>serial</t>
+  </si>
+  <si>
+    <t>hpc_partition</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>parallel</t>
   </si>
 </sst>
 </file>
@@ -366,7 +375,50 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -380,9 +432,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K50" totalsRowShown="0">
-  <autoFilter ref="A1:K50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L50" totalsRowShown="0">
+  <autoFilter ref="A1:L50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="hardware_utilization_strategy"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="device"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="run_mode"/>
@@ -390,6 +442,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="n_mpi_procs"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="n_omp_threads"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="n_gpus"/>
+    <tableColumn id="12" xr3:uid="{C4445796-869E-4847-856B-0EE8EE8365E5}" name="hpc_partition" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="total_MPI_ranks"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="total_OpenMP_threads"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="total_devices"/>
@@ -687,10 +740,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,13 +754,14 @@
     <col min="4" max="4" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="28.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,19 +784,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -764,24 +821,27 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H2" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I2" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>1</v>
       </c>
       <c r="J2" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -803,24 +863,27 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I3" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>4</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J3" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="K3" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="L3" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -842,24 +905,27 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="H4" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>8</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J4" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="K4" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K4" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="L4" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -881,24 +947,27 @@
       <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="H5" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H5" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>8</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J5" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="K5" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K5" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="L5" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -920,24 +989,27 @@
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="H6" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H6" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I6" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>16</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J6" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-      <c r="K6" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K6" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="L6" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -959,24 +1031,27 @@
       <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="H7" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H7" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I7" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>16</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J7" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-      <c r="K7" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K7" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="L7" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
@@ -998,24 +1073,27 @@
       <c r="G8" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H8" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I8" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>16</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J8" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-      <c r="K8" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K8" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="L8" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -1037,24 +1115,27 @@
       <c r="G9" s="6">
         <v>0</v>
       </c>
-      <c r="H9" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H9" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I9" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>32</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J9" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K9" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K9" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L9" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1076,24 +1157,27 @@
       <c r="G10" s="6">
         <v>0</v>
       </c>
-      <c r="H10" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I10" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>32</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J10" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K10" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K10" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L10" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1115,24 +1199,27 @@
       <c r="G11" s="6">
         <v>0</v>
       </c>
-      <c r="H11" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H11" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I11" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>32</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J11" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K11" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K11" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L11" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -1154,24 +1241,27 @@
       <c r="G12" s="6">
         <v>0</v>
       </c>
-      <c r="H12" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H12" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I12" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>32</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J12" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K12" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K12" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L12" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
@@ -1193,24 +1283,27 @@
       <c r="G13" s="6">
         <v>0</v>
       </c>
-      <c r="H13" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H13" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I13" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J13" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K13" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K13" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L13" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
@@ -1232,24 +1325,27 @@
       <c r="G14" s="6">
         <v>0</v>
       </c>
-      <c r="H14" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
+      <c r="H14" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I14" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="J14" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K14" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K14" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L14" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1271,24 +1367,27 @@
       <c r="G15" s="6">
         <v>0</v>
       </c>
-      <c r="H15" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H15" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I15" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J15" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K15" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K15" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L15" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>16</v>
       </c>
@@ -1310,24 +1409,27 @@
       <c r="G16" s="6">
         <v>0</v>
       </c>
-      <c r="H16" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H16" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I16" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J16" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K16" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K16" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L16" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
@@ -1349,24 +1451,27 @@
       <c r="G17" s="6">
         <v>0</v>
       </c>
-      <c r="H17" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H17" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I17" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J17" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K17" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K17" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L17" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
@@ -1388,24 +1493,27 @@
       <c r="G18" s="6">
         <v>0</v>
       </c>
-      <c r="H18" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H18" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I18" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="J18" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J18" s="7">
+      <c r="K18" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K18" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
@@ -1427,24 +1535,27 @@
       <c r="G19" s="6">
         <v>0</v>
       </c>
-      <c r="H19" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
+      <c r="H19" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I19" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="J19" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J19" s="7">
+      <c r="K19" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K19" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
@@ -1466,24 +1577,27 @@
       <c r="G20" s="6">
         <v>0</v>
       </c>
-      <c r="H20" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H20" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I20" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="J20" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J20" s="7">
+      <c r="K20" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K20" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>16</v>
       </c>
@@ -1505,24 +1619,27 @@
       <c r="G21" s="6">
         <v>0</v>
       </c>
-      <c r="H21" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
+      <c r="H21" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I21" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="J21" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J21" s="7">
+      <c r="K21" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K21" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>16</v>
       </c>
@@ -1544,24 +1661,27 @@
       <c r="G22" s="6">
         <v>0</v>
       </c>
-      <c r="H22" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H22" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I22" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="J22" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J22" s="7">
+      <c r="K22" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K22" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>16</v>
       </c>
@@ -1583,24 +1703,27 @@
       <c r="G23" s="6">
         <v>0</v>
       </c>
-      <c r="H23" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H23" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I23" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="J23" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J23" s="7">
+      <c r="K23" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K23" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>16</v>
       </c>
@@ -1622,24 +1745,27 @@
       <c r="G24" s="6">
         <v>0</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="I24" s="7">
+      <c r="J24" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J24" s="7">
+      <c r="K24" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K24" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
@@ -1661,24 +1787,27 @@
       <c r="G25" s="6">
         <v>0</v>
       </c>
-      <c r="H25" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H25" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I25" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="J25" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J25" s="7">
+      <c r="K25" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K25" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>16</v>
       </c>
@@ -1700,24 +1829,27 @@
       <c r="G26" s="6">
         <v>0</v>
       </c>
-      <c r="H26" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
+      <c r="H26" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I26" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="J26" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J26" s="7">
+      <c r="K26" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K26" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>16</v>
       </c>
@@ -1739,24 +1871,27 @@
       <c r="G27" s="6">
         <v>0</v>
       </c>
-      <c r="H27" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
+      <c r="H27" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I27" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="J27" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J27" s="7">
+      <c r="K27" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K27" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>16</v>
       </c>
@@ -1778,24 +1913,27 @@
       <c r="G28" s="6">
         <v>0</v>
       </c>
-      <c r="H28" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H28" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I28" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="J28" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J28" s="7">
+      <c r="K28" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K28" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1817,24 +1955,27 @@
       <c r="G29" s="6">
         <v>0</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="I29" s="7">
+      <c r="J29" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J29" s="7">
+      <c r="K29" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K29" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>16</v>
       </c>
@@ -1856,24 +1997,27 @@
       <c r="G30" s="6">
         <v>0</v>
       </c>
-      <c r="H30" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
+      <c r="H30" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I30" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="J30" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J30" s="7">
+      <c r="K30" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K30" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>16</v>
       </c>
@@ -1895,24 +2039,27 @@
       <c r="G31" s="6">
         <v>0</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="I31" s="7">
+      <c r="J31" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J31" s="7">
+      <c r="K31" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K31" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>16</v>
       </c>
@@ -1934,24 +2081,27 @@
       <c r="G32" s="6">
         <v>0</v>
       </c>
-      <c r="H32" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
+      <c r="H32" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I32" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="J32" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J32" s="7">
+      <c r="K32" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K32" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>11</v>
       </c>
@@ -1973,24 +2123,27 @@
       <c r="G33" s="6">
         <v>0</v>
       </c>
-      <c r="H33" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H33" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I33" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>2</v>
       </c>
       <c r="J33" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
-      </c>
-      <c r="K33" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>2</v>
+      </c>
+      <c r="K33" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="L33" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>11</v>
       </c>
@@ -2012,24 +2165,27 @@
       <c r="G34" s="6">
         <v>0</v>
       </c>
-      <c r="H34" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H34" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I34" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>4</v>
       </c>
       <c r="J34" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="K34" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="K34" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="L34" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2051,24 +2207,27 @@
       <c r="G35" s="6">
         <v>0</v>
       </c>
-      <c r="H35" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H35" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I35" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>8</v>
       </c>
       <c r="J35" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="K35" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K35" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="L35" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>11</v>
       </c>
@@ -2090,24 +2249,27 @@
       <c r="G36" s="6">
         <v>0</v>
       </c>
-      <c r="H36" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
+      <c r="H36" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I36" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>16</v>
       </c>
       <c r="J36" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-      <c r="K36" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K36" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="L36" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>11</v>
       </c>
@@ -2129,24 +2291,27 @@
       <c r="G37" s="6">
         <v>0</v>
       </c>
-      <c r="H37" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
+      <c r="H37" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I37" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>32</v>
       </c>
       <c r="J37" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K37" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K37" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L37" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>11</v>
       </c>
@@ -2168,24 +2333,27 @@
       <c r="G38" s="6">
         <v>0</v>
       </c>
-      <c r="H38" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
+      <c r="H38" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I38" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>64</v>
       </c>
       <c r="J38" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K38" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K38" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L38" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>11</v>
       </c>
@@ -2207,24 +2375,27 @@
       <c r="G39" s="6">
         <v>0</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="I39" s="7">
+      <c r="J39" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J39" s="7">
+      <c r="K39" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K39" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2246,24 +2417,27 @@
       <c r="G40" s="6">
         <v>0</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="I40" s="7">
+      <c r="J40" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J40" s="7">
+      <c r="K40" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K40" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>11</v>
       </c>
@@ -2285,24 +2459,27 @@
       <c r="G41" s="6">
         <v>0</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="7">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="I41" s="7">
+      <c r="J41" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J41" s="7">
+      <c r="K41" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K41" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>14</v>
       </c>
@@ -2324,24 +2501,27 @@
       <c r="G42" s="6">
         <v>0</v>
       </c>
-      <c r="H42" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H42" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I42" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>2</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J42" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
-      </c>
-      <c r="K42" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>2</v>
+      </c>
+      <c r="K42" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="L42" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>14</v>
       </c>
@@ -2363,24 +2543,27 @@
       <c r="G43" s="6">
         <v>0</v>
       </c>
-      <c r="H43" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H43" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I43" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>4</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J43" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="K43" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="K43" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="L43" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>14</v>
       </c>
@@ -2402,24 +2585,27 @@
       <c r="G44" s="6">
         <v>0</v>
       </c>
-      <c r="H44" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H44" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I44" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>8</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J44" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="K44" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K44" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="L44" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>14</v>
       </c>
@@ -2441,24 +2627,27 @@
       <c r="G45" s="6">
         <v>0</v>
       </c>
-      <c r="H45" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H45" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I45" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>16</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J45" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-      <c r="K45" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K45" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="L45" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>14</v>
       </c>
@@ -2480,24 +2669,27 @@
       <c r="G46" s="6">
         <v>0</v>
       </c>
-      <c r="H46" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H46" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I46" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>32</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J46" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-      <c r="K46" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K46" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="L46" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>14</v>
       </c>
@@ -2519,24 +2711,27 @@
       <c r="G47" s="6">
         <v>0</v>
       </c>
-      <c r="H47" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>1</v>
+      <c r="H47" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I47" s="7">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-        <v>64</v>
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J47" s="7">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-      <c r="K47" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
+      </c>
+      <c r="K47" s="7">
+        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+      <c r="L47" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>14</v>
       </c>
@@ -2558,24 +2753,27 @@
       <c r="G48" s="6">
         <v>0</v>
       </c>
-      <c r="H48" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>2</v>
+      <c r="H48" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I48" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="J48" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>128</v>
       </c>
-      <c r="J48" s="7">
+      <c r="K48" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>128</v>
       </c>
-      <c r="K48" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>14</v>
       </c>
@@ -2597,24 +2795,27 @@
       <c r="G49" s="6">
         <v>0</v>
       </c>
-      <c r="H49" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>4</v>
+      <c r="H49" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I49" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="J49" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>256</v>
       </c>
-      <c r="J49" s="7">
+      <c r="K49" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>256</v>
       </c>
-      <c r="K49" s="8">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="8">
+        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>14</v>
       </c>
@@ -2636,19 +2837,22 @@
       <c r="G50" s="6">
         <v>0</v>
       </c>
-      <c r="H50" s="7">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-        <v>8</v>
+      <c r="H50" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I50" s="7">
+        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="J50" s="7">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
         <v>512</v>
       </c>
-      <c r="J50" s="7">
+      <c r="K50" s="7">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
         <v>512</v>
       </c>
-      <c r="K50" s="8">
+      <c r="L50" s="8">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
feat: add n_nodes validation and verbose parameter to config
Add validation for n_nodes parameter across all run modes (serial, openmp,
mpi, hybrid, gpu) to ensure MPI processes >= nodes and prevent single tasks
from spanning multiple nodes. Add verbose parameter to load_norfolk_system_config
function to control download status messages.
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/benchmarking_uva_cpus.xlsx
+++ b/test_data/norfolk_coastal_flooding/benchmarking_uva_cpus.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05D8AA-6DB6-4E0D-B4C6-F71F57CF6F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-28920" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Summary"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="23">
   <si>
     <t>hardware_utilization_strategy</t>
   </si>
@@ -88,8 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,14 +130,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3f3f76"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3f3f3f"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -133,21 +151,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffcc"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffcc99"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -192,7 +210,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -225,7 +243,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -235,128 +253,89 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFc6c6c6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L50" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:L50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L44" totalsRowShown="0">
+  <autoFilter ref="A1:L44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn name="hardware_utilization_strategy" id="1"/>
-    <tableColumn name="device" id="2"/>
-    <tableColumn name="run_mode" id="3"/>
-    <tableColumn name="n_nodes" id="4"/>
-    <tableColumn name="n_mpi_procs" id="5"/>
-    <tableColumn name="n_omp_threads" id="6"/>
-    <tableColumn name="n_gpus" id="7"/>
-    <tableColumn name="hpc_ensemble_partition" id="8"/>
-    <tableColumn name="total_MPI_ranks" id="9"/>
-    <tableColumn name="total_OpenMP_threads" id="10"/>
-    <tableColumn name="total_devices" id="11"/>
-    <tableColumn name="devices_per_node" id="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="hardware_utilization_strategy"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="device"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="run_mode"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="n_nodes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="n_mpi_procs"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="n_omp_threads"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="n_gpus"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="hpc_ensemble_partition"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="total_MPI_ranks"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="total_OpenMP_threads"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="total_devices"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="devices_per_node"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -365,10 +344,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -406,71 +385,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,7 +477,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -521,11 +500,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -534,13 +513,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -550,7 +529,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -559,7 +538,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -568,7 +547,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -576,10 +555,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -644,31 +623,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="29.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="17" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="17" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="17" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -733,18 +713,22 @@
       </c>
       <c r="I2" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J2" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>1</v>
       </c>
       <c r="K2" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="L2" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -771,18 +755,22 @@
       </c>
       <c r="I3" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J3" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
       </c>
       <c r="K3" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="L3" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -809,18 +797,22 @@
       </c>
       <c r="I4" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J4" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
       </c>
       <c r="K4" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="L4" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -847,18 +839,22 @@
       </c>
       <c r="I5" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J5" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
       </c>
       <c r="K5" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="L5" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -885,18 +881,22 @@
       </c>
       <c r="I6" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J6" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
       </c>
       <c r="K6" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="L6" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -923,18 +923,22 @@
       </c>
       <c r="I7" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J7" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
       </c>
       <c r="K7" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="L7" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -961,18 +965,22 @@
       </c>
       <c r="I8" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J8" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
       </c>
       <c r="K8" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="L8" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -999,18 +1007,22 @@
       </c>
       <c r="I9" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J9" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K9" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L9" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1037,18 +1049,22 @@
       </c>
       <c r="I10" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J10" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K10" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L10" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1075,18 +1091,22 @@
       </c>
       <c r="I11" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J11" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K11" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L11" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1113,18 +1133,22 @@
       </c>
       <c r="I12" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J12" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K12" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L12" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1151,18 +1175,22 @@
       </c>
       <c r="I13" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J13" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K13" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L13" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1189,18 +1217,22 @@
       </c>
       <c r="I14" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="J14" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K14" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L14" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1227,18 +1259,22 @@
       </c>
       <c r="I15" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J15" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K15" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L15" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1265,18 +1301,22 @@
       </c>
       <c r="I16" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J16" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K16" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L16" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1303,18 +1343,22 @@
       </c>
       <c r="I17" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J17" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K17" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L17" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1341,18 +1385,22 @@
       </c>
       <c r="I18" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J18" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K18" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L18" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1379,18 +1427,22 @@
       </c>
       <c r="I19" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="J19" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K19" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L19" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1417,18 +1469,22 @@
       </c>
       <c r="I20" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J20" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K20" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L20" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
@@ -1455,18 +1511,22 @@
       </c>
       <c r="I21" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="J21" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K21" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L21" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1493,18 +1553,22 @@
       </c>
       <c r="I22" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J22" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K22" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L22" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -1518,10 +1582,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="8">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F23" s="8">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G23" s="8">
         <v>0</v>
@@ -1531,18 +1595,22 @@
       </c>
       <c r="I23" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="J23" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>256</v>
       </c>
       <c r="K23" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="L23" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1556,10 +1624,10 @@
         <v>4</v>
       </c>
       <c r="E24" s="8">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F24" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G24" s="8">
         <v>0</v>
@@ -1569,18 +1637,22 @@
       </c>
       <c r="I24" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J24" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>256</v>
       </c>
       <c r="K24" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="L24" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1594,10 +1666,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="8">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F25" s="8">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G25" s="8">
         <v>0</v>
@@ -1607,18 +1679,22 @@
       </c>
       <c r="I25" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="J25" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>256</v>
       </c>
       <c r="K25" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="L25" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1632,10 +1708,10 @@
         <v>4</v>
       </c>
       <c r="E26" s="8">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F26" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G26" s="8">
         <v>0</v>
@@ -1645,18 +1721,22 @@
       </c>
       <c r="I26" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="J26" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>256</v>
       </c>
       <c r="K26" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="L26" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1667,13 +1747,13 @@
         <v>17</v>
       </c>
       <c r="D27" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27" s="8">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F27" s="8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G27" s="8">
         <v>0</v>
@@ -1683,18 +1763,22 @@
       </c>
       <c r="I27" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="J27" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>512</v>
       </c>
       <c r="K27" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>512</v>
       </c>
       <c r="L27" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>16</v>
       </c>
@@ -1708,10 +1792,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F28" s="8">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G28" s="8">
         <v>0</v>
@@ -1721,18 +1805,22 @@
       </c>
       <c r="I28" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="J28" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>512</v>
       </c>
       <c r="K28" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>512</v>
       </c>
       <c r="L28" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
@@ -1746,10 +1834,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="8">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F29" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G29" s="8">
         <v>0</v>
@@ -1759,132 +1847,148 @@
       </c>
       <c r="I29" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="J29" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>512</v>
       </c>
       <c r="K29" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>512</v>
       </c>
       <c r="L29" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D30" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E30" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" s="8">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G30" s="8">
         <v>0</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I30" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="J30" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>2</v>
       </c>
       <c r="K30" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="L30" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D31" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E31" s="8">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F31" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G31" s="8">
         <v>0</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I31" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="J31" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
       </c>
       <c r="K31" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="L31" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D32" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E32" s="8">
         <v>8</v>
       </c>
       <c r="F32" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G32" s="8">
         <v>0</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I32" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="J32" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
       </c>
       <c r="K32" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="L32" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>19</v>
       </c>
@@ -1898,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F33" s="8">
         <v>1</v>
@@ -1911,18 +2015,22 @@
       </c>
       <c r="I33" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="J33" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
       </c>
       <c r="K33" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="L33" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
@@ -1936,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="8">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F34" s="8">
         <v>1</v>
@@ -1949,18 +2057,22 @@
       </c>
       <c r="I34" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="J34" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K34" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L34" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
@@ -1974,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="8">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="F35" s="8">
         <v>1</v>
@@ -1987,18 +2099,22 @@
       </c>
       <c r="I35" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="J35" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K35" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L35" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>19</v>
       </c>
@@ -2009,10 +2125,10 @@
         <v>20</v>
       </c>
       <c r="D36" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="8">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F36" s="8">
         <v>1</v>
@@ -2021,22 +2137,26 @@
         <v>0</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I36" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="J36" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>128</v>
       </c>
       <c r="K36" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>128</v>
       </c>
       <c r="L36" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
@@ -2047,10 +2167,10 @@
         <v>20</v>
       </c>
       <c r="D37" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E37" s="8">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F37" s="8">
         <v>1</v>
@@ -2059,22 +2179,26 @@
         <v>0</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I37" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="J37" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>256</v>
       </c>
       <c r="K37" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>256</v>
       </c>
       <c r="L37" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -2085,7 +2209,7 @@
         <v>20</v>
       </c>
       <c r="D38" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E38" s="8">
         <v>64</v>
@@ -2097,136 +2221,152 @@
         <v>0</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I38" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>512</v>
       </c>
       <c r="J38" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>512</v>
       </c>
       <c r="K38" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>512</v>
       </c>
       <c r="L38" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D39" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="8">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F39" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39" s="8">
         <v>0</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I39" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J39" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>2</v>
       </c>
       <c r="K39" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>2</v>
       </c>
       <c r="L39" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D40" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E40" s="8">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F40" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G40" s="8">
         <v>0</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I40" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J40" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>4</v>
       </c>
       <c r="K40" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>4</v>
       </c>
       <c r="L40" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D41" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E41" s="8">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F41" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G41" s="8">
         <v>0</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I41" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J41" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>8</v>
       </c>
       <c r="K41" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>8</v>
       </c>
       <c r="L41" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>21</v>
       </c>
@@ -2243,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G42" s="8">
         <v>0</v>
@@ -2253,18 +2393,22 @@
       </c>
       <c r="I42" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J42" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>16</v>
       </c>
       <c r="K42" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>16</v>
       </c>
       <c r="L42" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -2281,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="8">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G43" s="8">
         <v>0</v>
@@ -2291,18 +2435,22 @@
       </c>
       <c r="I43" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J43" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>32</v>
       </c>
       <c r="K43" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>32</v>
       </c>
       <c r="L43" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>21</v>
       </c>
@@ -2319,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="8">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="G44" s="8">
         <v>0</v>
@@ -2329,243 +2477,19 @@
       </c>
       <c r="I44" s="10">
         <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>1</v>
       </c>
       <c r="J44" s="10">
         <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
+        <v>64</v>
       </c>
       <c r="K44" s="10">
         <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
       <c r="L44" s="11">
         <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="8">
-        <v>1</v>
-      </c>
-      <c r="E45" s="8">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
-        <v>16</v>
-      </c>
-      <c r="G45" s="8">
-        <v>0</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J45" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K45" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L45" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="8">
-        <v>1</v>
-      </c>
-      <c r="E46" s="8">
-        <v>1</v>
-      </c>
-      <c r="F46" s="8">
-        <v>32</v>
-      </c>
-      <c r="G46" s="8">
-        <v>0</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I46" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J46" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K46" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L46" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="8">
-        <v>1</v>
-      </c>
-      <c r="E47" s="8">
-        <v>1</v>
-      </c>
-      <c r="F47" s="8">
-        <v>64</v>
-      </c>
-      <c r="G47" s="8">
-        <v>0</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J47" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K47" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L47" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="8">
-        <v>2</v>
-      </c>
-      <c r="E48" s="8">
-        <v>1</v>
-      </c>
-      <c r="F48" s="8">
-        <v>64</v>
-      </c>
-      <c r="G48" s="8">
-        <v>0</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J48" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K48" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L48" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="8">
-        <v>4</v>
-      </c>
-      <c r="E49" s="8">
-        <v>1</v>
-      </c>
-      <c r="F49" s="8">
-        <v>64</v>
-      </c>
-      <c r="G49" s="8">
-        <v>0</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J49" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K49" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L49" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="14">
-        <v>8</v>
-      </c>
-      <c r="E50" s="14">
-        <v>1</v>
-      </c>
-      <c r="F50" s="14">
-        <v>64</v>
-      </c>
-      <c r="G50" s="8">
-        <v>0</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="10">
-        <f>Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="J50" s="10">
-        <f>Table1[[#This Row], [total_MPI_ranks]]*Table1[[#This Row], [n_omp_threads]]</f>
-      </c>
-      <c r="K50" s="10">
-        <f>Table1[[#This Row], [n_omp_threads]]*Table1[[#This Row], [n_mpi_procs]]*Table1[[#This Row], [n_nodes]]</f>
-      </c>
-      <c r="L50" s="11">
-        <f>Table1[[#This Row], [total_devices]]/Table1[[#This Row], [n_nodes]]</f>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>